<commit_message>
Added listeners and updated tests
</commit_message>
<xml_diff>
--- a/src/test/java/com/chinmay/resources/Data.xlsx
+++ b/src/test/java/com/chinmay/resources/Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>uname</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Count</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -63,6 +60,21 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/auth/login</t>
   </si>
 </sst>
 </file>
@@ -430,7 +442,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -479,7 +491,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -490,20 +502,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -511,13 +524,19 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -525,13 +544,19 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -539,13 +564,19 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -553,13 +584,19 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -567,10 +604,16 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added remote webdriver support
</commit_message>
<xml_diff>
--- a/src/test/java/com/chinmay/resources/Data.xlsx
+++ b/src/test/java/com/chinmay/resources/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>uname</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>https://opensource-demo.orangehrmlive.com/web/index.php/auth/login</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>remote</t>
   </si>
 </sst>
 </file>
@@ -441,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -502,21 +511,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -530,13 +539,16 @@
         <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -550,13 +562,16 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -570,13 +585,16 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -590,13 +608,16 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -610,9 +631,12 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>